<commit_message>
finished following and liking
code is clean but liking has a little bug
</commit_message>
<xml_diff>
--- a/followed_users.xlsx
+++ b/followed_users.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -345,59 +344,155 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.6"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>hello</t>
+          <t>alash_arts</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>world!</t>
+          <t>01/09/2020, 11:59:37</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>hallo</t>
+          <t>lolariostyle</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>welt</t>
+          <t>01/09/2020, 11:59:50</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>z1n.__.01</t>
+          <t>yleniastorti</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>01/09/2020, 11:44:05</t>
+          <t>01/09/2020, 12:06:04</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>swissmonamour</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:06:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>fashiongirls91</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:06:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mesiszigeti</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:06:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>lolariostyle</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>01/09/2020, 11:44:18</t>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:22:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fashiongirls91</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:23:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>mesiszigeti</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:23:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ikizlerlekurabiyeler</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:31:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>_.fayis2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:31:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>italia_dev</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>01/09/2020, 12:31:42</t>
         </is>
       </c>
     </row>

</xml_diff>